<commit_message>
adding solved version's of Saturdays student activities
</commit_message>
<xml_diff>
--- a/01-Excel/Saturday/Activities/03-Stu_LineAndBar/Unsolved/StudentGrades_Unsolved.xlsx
+++ b/01-Excel/Saturday/Activities/03-Stu_LineAndBar/Unsolved/StudentGrades_Unsolved.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\3\Activities\03-Stu_LineAndBar\Unsolved\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gweathersby\Documents\Backup_10_18_2015\Personal\GA Tech\GTATL201808DATA3\01-Excel\Saturday\Activities\03-Stu_LineAndBar\Unsolved\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -158,6 +158,2986 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aleisha Lavine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-165C-438D-8EE4-7EA770F4F02B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="422944832"/>
+        <c:axId val="422945160"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Tad Ethridge</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$2:$G$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>63</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Veda Sanon</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$3:$G$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>57</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>76</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>67</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Timothy Trimm</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$4:$G$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>76</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>77</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>82</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>85</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Odelia Nelsen</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$5:$G$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>97</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>99</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>93</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>94</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>99</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Danica Nygard</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$7:$G$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>73</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>79</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Chadwick Eagle</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$8:$G$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>25</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Petra Mulvey</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$9:$G$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>52</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="8"/>
+                <c:order val="8"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Nannette Dafoe</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$10:$G$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>92</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>88</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>98</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000008-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="9"/>
+                <c:order val="9"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Jaye Cartier</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$11:$G$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>93</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>97</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>95</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000009-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="10"/>
+                <c:order val="10"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Cora Stolle</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$12:$G$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>77</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>81</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>81</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000A-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="11"/>
+                <c:order val="11"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Amado Tawney</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$13:$G$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>58</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>58</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000B-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="12"/>
+                <c:order val="12"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Jeremiah Muncy</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$14:$G$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>57</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>50</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000C-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="13"/>
+                <c:order val="13"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$15</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Kathe Gallivan</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$15:$G$15</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>33</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000D-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="14"/>
+                <c:order val="14"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Wilfred Gasca</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$16:$G$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>92</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>82</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>75</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000E-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="15"/>
+                <c:order val="15"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$17</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Cristobal Hogans</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$17:$G$17</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>55</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>73</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>73</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000F-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="16"/>
+                <c:order val="16"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$18</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Milton Tubb</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$18:$G$18</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>70</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000010-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="17"/>
+                <c:order val="17"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Kattie Buttars</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$19:$G$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>53</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000011-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="18"/>
+                <c:order val="18"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Milford Kennan</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="80000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$20:$G$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>98</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>95</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000012-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="19"/>
+                <c:order val="19"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Meghan Donaldson</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="80000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Jan</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Feb</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Mar</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Apr</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>May</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Jun</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$21:$G$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>27</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000013-165C-438D-8EE4-7EA770F4F02B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="422944832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422945160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="422945160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422944832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>186765</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>141193</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276412</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>186763</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C108E3D1-EFCD-4C9E-98A7-6EDE2BC264AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -460,16 +3440,16 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="12" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="2" max="12" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>20</v>
       </c>
@@ -489,7 +3469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +3497,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -545,7 +3525,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -573,7 +3553,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -601,7 +3581,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -629,7 +3609,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -657,7 +3637,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -685,7 +3665,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -713,7 +3693,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -741,7 +3721,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -769,7 +3749,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -797,7 +3777,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -825,7 +3805,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -853,7 +3833,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -881,7 +3861,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -909,7 +3889,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -937,7 +3917,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -965,7 +3945,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -993,7 +3973,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1021,7 +4001,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1051,5 +4031,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>